<commit_message>
Fixed data of excel
</commit_message>
<xml_diff>
--- a/data/BOOKSGENRES.xlsx
+++ b/data/BOOKSGENRES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TN3Vocab\EnglishTN3Vocab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2C7087B-DB4A-4E1C-A1DC-5F534B4294CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC983759-CD76-47FA-809B-C483D003A81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1AA47019-26BE-49AA-9C84-C1FDF0F07AC5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>novel (n)</t>
   </si>
@@ -90,16 +90,280 @@
     <t>self-help</t>
   </si>
   <si>
-    <t>sách tự lực (chia sẻ các tips trong đời sống)</t>
-  </si>
-  <si>
     <t>Từ vựng / Cụm từ (English)</t>
   </si>
   <si>
-    <t>Nghĩa / Giải thích (Vietnamese/English)</t>
-  </si>
-  <si>
-    <t>Examples</t>
+    <t>Nghĩa / Giải thích (Vietnamese)</t>
+  </si>
+  <si>
+    <t>Examples (Ví dụ)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"Harry Potter" is a famous fantasy </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>novel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">She loves reading a good </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>mystery</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> before bed.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The movie was a psychological </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>thriller</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> that kept us guessing.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">My grandmother enjoys reading a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>romance novel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> on the weekend.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"Dune" is a classic </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>science fiction book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">He published a collection of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>short stories</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I am reading a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>biography</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> of Albert Einstein.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In his </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>autobiography</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, he describes his childhood struggles.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>travel book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> lists the best hotels in Paris.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The former president wrote his </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>memoirs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> after leaving office.</t>
+    </r>
+  </si>
+  <si>
+    <t>sách tự lực</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">She bought a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>self-help</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> book to improve her confidence.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -115,17 +379,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,17 +409,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
+      <left style="medium">
+        <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
+      <right style="medium">
+        <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -163,13 +427,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,125 +752,147 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>